<commit_message>
Able to handle one type of format
</commit_message>
<xml_diff>
--- a/message_0_WillsData.xlsx
+++ b/message_0_WillsData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,47 +436,57 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>first_name</t>
+          <t>email</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>last_name</t>
+          <t>name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>lastname</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>gender</t>
+          <t>adress</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ip_address</t>
+          <t>city</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>car_VIN</t>
+          <t>state</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>city</t>
+          <t>zip</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>credit_card</t>
+          <t>phone</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>street_address</t>
+          <t>dob</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ssn</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>dl or id</t>
         </is>
       </c>
     </row>
@@ -486,47 +496,57 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Arny</t>
+          <t>curtis_smith256@yahoo.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Gibbeson</t>
+          <t>CURTIS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>agibbeson0@answers.com</t>
+          <t>SMITH</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Bigender</t>
+          <t>3948 FLEMING WAY</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>244.151.89.48</t>
+          <t>ASHBURN</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3VW4T7AT7EM832849</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Vilufushi</t>
+          <t>20148</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>3572142955447349</t>
+          <t>7037246123</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>69 Maple Wood Center</t>
+          <t>1954-05-08</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>231669540</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>03SHC8121496</t>
         </is>
       </c>
     </row>
@@ -536,47 +556,57 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kym</t>
+          <t>ctucker@comcast.net</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Coward</t>
+          <t>CHARLES</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>kcoward1@pbs.org</t>
+          <t>TUCKER</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Genderfluid</t>
+          <t>2174 COLUMBIA MINE RD</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.114.30.127</t>
+          <t>CLARKSBURG</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5N1AA0NC5BN566080</t>
+          <t>WV</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Banepa</t>
+          <t>26301</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>5018131477431920</t>
+          <t>3048388674</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>31 Emmet Road</t>
+          <t>1988-03-05</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>234334988</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>T26011586540</t>
         </is>
       </c>
     </row>
@@ -586,47 +616,57 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ronny</t>
+          <t>curtisriggs33@yahoo.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Leverich</t>
+          <t>CURTIS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>rleverich2@sbwire.com</t>
+          <t>RIGGS</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Non-binary</t>
+          <t>1427 POPLAR ST APT 12</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11.36.102.5</t>
+          <t>PITTSBURGH</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>SCFBB03B37G622353</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Kapuan</t>
+          <t>15205</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>5150708743105574</t>
+          <t>4128052281</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>7562 Harbort Terrace</t>
+          <t>1963-08-09</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>235297200</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>29990512</t>
         </is>
       </c>
     </row>
@@ -636,47 +676,57 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Carmon</t>
+          <t>cuffieangela@hotmail.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Runacres</t>
+          <t>ANGELA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>crunacres3@newyorker.com</t>
+          <t>CUFFIE</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>410 N 14TH ST APT A</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>248.71.36.38</t>
+          <t>EAST SAINT LOUIS</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>WAUBVAFB6AN542276</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Jemielno</t>
+          <t>62201</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>3560218518388321</t>
+          <t>6184478720</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>8 5th Alley</t>
+          <t>1950-01-13</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>237415525</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>10001779847C</t>
         </is>
       </c>
     </row>
@@ -686,47 +736,57 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Britney</t>
+          <t>curtiscameron17@gmail.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Rossander</t>
+          <t>SAMUEL</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>brossander4@xing.com</t>
+          <t>CAMERON</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Genderqueer</t>
+          <t>533 GOSPEL LN</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>163.141.242.158</t>
+          <t>SEVIERVILLE</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1J4PR4GK3AC135342</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Karamat</t>
+          <t>37876</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>3573693403544649</t>
+          <t>8652569288</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>5 Debs Court</t>
+          <t>1991-06-22</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>237511899</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>21881270</t>
         </is>
       </c>
     </row>
@@ -736,47 +796,57 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Quill</t>
+          <t>curtisdnorman@yahoo.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tupling</t>
+          <t>CURTIS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>qtupling5@studiopress.com</t>
+          <t>NORMAN</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Genderfluid</t>
+          <t>2410 OLD STEINE RD APT 801</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>60.144.16.105</t>
+          <t>CHARLOTTE</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>WBAYF4C50FG089405</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Houyu</t>
+          <t>28269</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>3534796395924063</t>
+          <t>3365416404</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>88877 Westridge Center</t>
+          <t>1984-11-10</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>238418768</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>26831736</t>
         </is>
       </c>
     </row>
@@ -786,47 +856,57 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nicole</t>
+          <t>curtis.sifford@yahoo.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Jon</t>
+          <t>CURTIS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>njon6@cmu.edu</t>
+          <t>SIFFORD</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>2233 PREAKNESS CT</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>11.199.69.25</t>
+          <t>CHARLOTTE</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>WAUJT64B73N836631</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Cabrela</t>
+          <t>28273</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3542995225410927</t>
+          <t>7043943894</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>5 Hovde Road</t>
+          <t>2/28/1976 0:00</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>239418618</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>4524561</t>
         </is>
       </c>
     </row>
@@ -836,47 +916,57 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Maximilianus</t>
+          <t>ctjenkins82@yahoo.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Adess</t>
+          <t>CHARLES</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>madess7@newyorker.com</t>
+          <t>JENKINS</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Genderfluid</t>
+          <t>605 EDGEWOOD AVE</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>20.175.193.134</t>
+          <t>THOMASVILLE</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1FMHK7B81BG404372</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Rongxiang</t>
+          <t>27360</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>633348740698057056</t>
+          <t>3362253178</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>3394 Nelson Street</t>
+          <t>1977-01-24</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>239490946</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>29348438</t>
         </is>
       </c>
     </row>
@@ -886,47 +976,57 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cordi</t>
+          <t>ctyoung2012@gmail.com</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Brislawn</t>
+          <t>CHRISTOPHE</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>cbrislawn8@networksolutions.com</t>
+          <t>YOUNG</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>402 LASSITER DR</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>71.188.122.207</t>
+          <t>HIGH POINT</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>SCFEFBAC1AG811762</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Neuilly-sur-Marne</t>
+          <t>27265</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>374622161877104</t>
+          <t>3366875495</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>8 Sachtjen Alley</t>
+          <t>1967-02-02</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>239614829</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>29788463</t>
         </is>
       </c>
     </row>
@@ -936,47 +1036,57 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Marne</t>
+          <t>ctoya07@yahoo.com</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Oosthout de Vree</t>
+          <t>LATOYA</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>moosthoutdevree9@google.cn</t>
+          <t>CADE</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Non-binary</t>
+          <t>2544 BALTIMORE RD</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>191.213.56.71</t>
+          <t>BOLTON</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>WAULC68E43A467375</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Lingshan</t>
+          <t>28423</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>5108750890270507</t>
+          <t>9106409019</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>8664 Atwood Lane</t>
+          <t>1974-12-03</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>239638487</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>27990649</t>
         </is>
       </c>
     </row>
@@ -986,47 +1096,57 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Pepillo</t>
+          <t>ctl102574032@centurylink.net</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Dimmock</t>
+          <t>JOHN</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>pdimmocka@house.gov</t>
+          <t>JONES</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Genderqueer</t>
+          <t>1906 BRANDYWINE CT</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10.244.178.59</t>
+          <t>FAYETTEVILLE</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1GYS3BKJ4FR211184</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Ciparay</t>
+          <t>28304</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>6375009974733052</t>
+          <t>9107297209</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>4692 Northridge Hill</t>
+          <t>1975-06-06</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>239716848</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>34429957</t>
         </is>
       </c>
     </row>
@@ -1036,47 +1156,57 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Denny</t>
+          <t>cuddlehuddle2009@yahoo.com</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>McKague</t>
+          <t>HEATHER</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>dmckagueb@myspace.com</t>
+          <t>JEWELL</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Genderfluid</t>
+          <t>519 ELAND DR</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>75.161.4.104</t>
+          <t>NORTH FORT MYERS</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>5GAKVAED2BJ510716</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Novosibirsk</t>
+          <t>33917</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3565624314413004</t>
+          <t>2396562076</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>962 Jackson Park</t>
+          <t>1957-02-06</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>239889550</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>J40032488746</t>
         </is>
       </c>
     </row>
@@ -1086,47 +1216,1137 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Felecia</t>
+          <t>curtisruffin@yahoo.com</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Audley</t>
+          <t>CURTIS</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>faudleyc@unesco.org</t>
+          <t>RUFFIN</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Non-binary</t>
+          <t>1017 BRINGLE FERRY RD</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>4.230.27.159</t>
+          <t>SALISBURY</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1FTSW3A58AE106054</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Cawayan</t>
+          <t>28144</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>3552004988187462</t>
+          <t>7046136744</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>4 Bobwhite Place</t>
+          <t>1967-01-29</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>241391002</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>24270400</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>cunninghamantonette@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CHRYSTALON</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>WEBBER</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>76 WHITE FAWN DR</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ASHEVILLE</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>28801</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>8282588367</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>9/9/1980 0:00</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>242352091</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>26628838</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>curtisblo44@gmail.com</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CURTIS</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>EDWARDS</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2750 REBECCA LN</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>KINSTON</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>28504</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2522860440</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>1974-03-28</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>242373464</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>24351004</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>cuadahyhallur@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CAUDAHY</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>HALL</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>434 W ARROWOOD RD</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>CHARLOTTE</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>28217</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>7043450653</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>1958-11-07</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>242659265</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>27563115</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>curlz22000@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>CURTIS</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>FIELDS</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1015 FOX HUNT LN APT B</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>RALEIGH</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>27615</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2524681206</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>1984-10-05</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>243517929</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>24579125</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ctmt7122@gmail.com</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>COURTNEY</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>TAYLOR</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>712 RIDGEWORTH AVE</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>HIGH POINT</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>27265</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>3369914002</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>1984-12-12</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>243550463</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>26632376</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>curtisandrews21@ymail.com</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>CURTIS</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>ANDREWS</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>4819 SILVER BRIAE</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>GREENSBORO</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>27410</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3369874288</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>1979-09-29</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>243595505</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>34208688</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>curlycueluvsyou@aol.com</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>BROOKE</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>STAMEY</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>125 WILD MEADOWS RD</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>FRANKLIN</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>28734</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>8284219734</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>1988-08-27</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>243710286</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>37533648</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>curreycrouch@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CURREY</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>CROUCH</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>115 REDFEARN WAY</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>JEFFERSON</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>29718</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>8436723069</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>1948-03-18</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>244392629</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>101824110</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>currymichael3436@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>MICHAEL</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>CURRY</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>216 HEATHER LN</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>CHERRYVILLE</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>28021</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>7044356213</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>4/2/1976 0:00</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>244491539</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>9805137</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>curryevette@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>EVETTE</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>CURRY</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>405 OVERTON PLACE</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>FAYETTEVILLE</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>28303</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>9104761874</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>3/8/1986 0:00</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>244593467</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>28384666</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>cumatthews@comcast.net</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>CURTIS</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>MATTHEWS</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1470 WATSON LN</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>FAYETTEVILLE</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>28311</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>9107792453</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>1962-01-25</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>244706972</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>M32011085284</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ctisdale80@gmail.com</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CARLOS</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>TISDALE</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>3185 CHESTNUT ST</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>LORIS</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>29569</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>9109181481</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>1969-08-03</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>245450972</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>101365940</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>cub_6606@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>CLIFTON</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>CUTHBERTSON</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>135 MCKINNEY ST</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>RUTHERFORDTON</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>28139</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>8282898668</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>1974-01-17</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>245650342</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>21474948</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>cudablue1218@gmail.com</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>GREGORY</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>LIVENGOOD</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>811 KLONDALE AVE</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>KANNAPOLIS</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>28081</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>7042734256</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>1973-11-02</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>245652027</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>24837742</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>curiouscrs@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>CATRINA</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>SMALLS</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>6407 MATLEA CT</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>CHARLOTTE</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>28215</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>7044005247</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>1988-06-04</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>247619525</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>7705263</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>cunninghamterry62@ymail.com</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>TERRY</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>CUNNIGHAM</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>121 HAROLDS PARK</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>CLINTON</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>29325</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>8645475219</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>1968-05-19</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>247658867</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>100403208</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>curtis4429@att.net</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>DOROTHY</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>ROACH</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>1019 SADDLE CLUB RD</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>RIDGEWAY</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>29130</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>8032061160</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>0114-02-04</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>247732621</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>7863928</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>cunninghamsequoia@yahoo.com</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>SEQUOIA</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>CUNNINGHAM</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>1133 SPRINGDALE RD APT 104</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>ROCK HILL</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>29730</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>8644353771</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>1957-05-30</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>247873083</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>101686071</t>
         </is>
       </c>
     </row>

</xml_diff>